<commit_message>
Minor cleanup of TE consensus tables
</commit_message>
<xml_diff>
--- a/TE_class_complexes_consensus.xlsx
+++ b/TE_class_complexes_consensus.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhlub\Documents\khare_lab\coronavirus (1)\new_variants\omicron\upload\omicron_models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{85C04D28-EEE3-4664-9CF7-82AF713088F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C78371F-832D-4EEE-9E85-A14E34818930}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="-24360" yWindow="4440" windowWidth="11175" windowHeight="6945" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="antibody_class_models_identific" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="881" uniqueCount="584">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="869" uniqueCount="583">
   <si>
     <t>Therapeutic Entity</t>
   </si>
@@ -620,9 +620,6 @@
   </si>
   <si>
     <t>S2L20</t>
-  </si>
-  <si>
-    <t>NTD</t>
   </si>
   <si>
     <t>4A8</t>
@@ -1780,7 +1777,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -4161,12 +4158,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P287"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
+      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4198,10 +4195,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="183" t="s">
+        <v>392</v>
+      </c>
+      <c r="E1" s="183" t="s">
         <v>393</v>
-      </c>
-      <c r="E1" s="183" t="s">
-        <v>394</v>
       </c>
       <c r="F1" s="183" t="s">
         <v>3</v>
@@ -4248,7 +4245,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="181" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="E2" s="180">
         <v>7</v>
@@ -4298,7 +4295,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="E3" s="4">
         <v>6</v>
@@ -4348,7 +4345,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="E4" s="6">
         <v>5</v>
@@ -4398,7 +4395,7 @@
         <v>1</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="E5" s="8">
         <v>5</v>
@@ -4448,7 +4445,7 @@
         <v>1</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="E6" s="10">
         <v>5</v>
@@ -4498,7 +4495,7 @@
         <v>1</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="E7" s="12">
         <v>5</v>
@@ -4537,7 +4534,7 @@
         <v>0.42499999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="193" t="s">
         <v>21</v>
       </c>
@@ -4548,7 +4545,7 @@
         <v>1</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E8" s="14">
         <v>4</v>
@@ -4598,7 +4595,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="E9" s="16">
         <v>4</v>
@@ -4648,7 +4645,7 @@
         <v>1</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="E10" s="18">
         <v>4</v>
@@ -4698,7 +4695,7 @@
         <v>1</v>
       </c>
       <c r="D11" s="21" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E11" s="20">
         <v>3</v>
@@ -4748,7 +4745,7 @@
         <v>1</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E12" s="22">
         <v>3</v>
@@ -4798,7 +4795,7 @@
         <v>1</v>
       </c>
       <c r="D13" s="25" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="E13" s="24">
         <v>3</v>
@@ -4848,7 +4845,7 @@
         <v>1</v>
       </c>
       <c r="D14" s="27" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="E14" s="26">
         <v>3</v>
@@ -4898,7 +4895,7 @@
         <v>1</v>
       </c>
       <c r="D15" s="29" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="E15" s="28">
         <v>2</v>
@@ -4948,7 +4945,7 @@
         <v>1</v>
       </c>
       <c r="D16" s="31" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="E16" s="30">
         <v>2</v>
@@ -4998,7 +4995,7 @@
         <v>1</v>
       </c>
       <c r="D17" s="33" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="E17" s="32">
         <v>2</v>
@@ -5048,7 +5045,7 @@
         <v>1</v>
       </c>
       <c r="D18" s="35" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="E18" s="34">
         <v>2</v>
@@ -5098,7 +5095,7 @@
         <v>1</v>
       </c>
       <c r="D19" s="37" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E19" s="36">
         <v>2</v>
@@ -5148,7 +5145,7 @@
         <v>1</v>
       </c>
       <c r="D20" s="39" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="E20" s="38">
         <v>2</v>
@@ -5198,7 +5195,7 @@
         <v>1</v>
       </c>
       <c r="D21" s="37" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="E21" s="36">
         <v>2</v>
@@ -5248,7 +5245,7 @@
         <v>1</v>
       </c>
       <c r="D22" s="41" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="E22" s="40">
         <v>2</v>
@@ -5298,7 +5295,7 @@
         <v>1</v>
       </c>
       <c r="D23" s="43" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E23" s="42">
         <v>2</v>
@@ -5348,7 +5345,7 @@
         <v>1</v>
       </c>
       <c r="D24" s="45" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="E24" s="44">
         <v>2</v>
@@ -5398,7 +5395,7 @@
         <v>1</v>
       </c>
       <c r="D25" s="47" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="E25" s="46">
         <v>2</v>
@@ -6248,7 +6245,7 @@
         <v>2</v>
       </c>
       <c r="D42" s="13" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="E42" s="12">
         <v>18</v>
@@ -6298,7 +6295,7 @@
         <v>2</v>
       </c>
       <c r="D43" s="63" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="E43" s="62">
         <v>18</v>
@@ -6348,7 +6345,7 @@
         <v>2</v>
       </c>
       <c r="D44" s="65" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="E44" s="64">
         <v>13</v>
@@ -6398,7 +6395,7 @@
         <v>2</v>
       </c>
       <c r="D45" s="67" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="E45" s="66">
         <v>9</v>
@@ -6448,7 +6445,7 @@
         <v>2</v>
       </c>
       <c r="D46" s="69" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="E46" s="68">
         <v>9</v>
@@ -6498,7 +6495,7 @@
         <v>2</v>
       </c>
       <c r="D47" s="71" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="E47" s="70">
         <v>8</v>
@@ -6548,7 +6545,7 @@
         <v>2</v>
       </c>
       <c r="D48" s="73" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="E48" s="72">
         <v>7</v>
@@ -6598,7 +6595,7 @@
         <v>2</v>
       </c>
       <c r="D49" s="71" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E49" s="70">
         <v>6</v>
@@ -6648,7 +6645,7 @@
         <v>2</v>
       </c>
       <c r="D50" s="75" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E50" s="74">
         <v>6</v>
@@ -6687,7 +6684,7 @@
         <v>1.0208333333333299</v>
       </c>
     </row>
-    <row r="51" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A51" s="224" t="s">
         <v>80</v>
       </c>
@@ -6698,7 +6695,7 @@
         <v>2</v>
       </c>
       <c r="D51" s="77" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="E51" s="76">
         <v>4</v>
@@ -6748,7 +6745,7 @@
         <v>2</v>
       </c>
       <c r="D52" s="79" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E52" s="78">
         <v>3</v>
@@ -6798,7 +6795,7 @@
         <v>2</v>
       </c>
       <c r="D53" s="69" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="E53" s="68">
         <v>3</v>
@@ -6848,7 +6845,7 @@
         <v>2</v>
       </c>
       <c r="D54" s="37" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="E54" s="36">
         <v>3</v>
@@ -6898,7 +6895,7 @@
         <v>2</v>
       </c>
       <c r="D55" s="81" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="E55" s="80">
         <v>3</v>
@@ -6948,7 +6945,7 @@
         <v>2</v>
       </c>
       <c r="D56" s="83" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E56" s="82">
         <v>3</v>
@@ -6998,7 +6995,7 @@
         <v>2</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="E57" s="2">
         <v>3</v>
@@ -7048,7 +7045,7 @@
         <v>2</v>
       </c>
       <c r="D58" s="85" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="E58" s="84">
         <v>3</v>
@@ -7098,7 +7095,7 @@
         <v>2</v>
       </c>
       <c r="D59" s="49" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="E59" s="48">
         <v>3</v>
@@ -7148,7 +7145,7 @@
         <v>2</v>
       </c>
       <c r="D60" s="87" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="E60" s="86">
         <v>3</v>
@@ -7198,7 +7195,7 @@
         <v>2</v>
       </c>
       <c r="D61" s="59" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="E61" s="58">
         <v>3</v>
@@ -7248,7 +7245,7 @@
         <v>2</v>
       </c>
       <c r="D62" s="81" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="E62" s="80">
         <v>3</v>
@@ -7298,7 +7295,7 @@
         <v>2</v>
       </c>
       <c r="D63" s="89" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="E63" s="88">
         <v>3</v>
@@ -7348,7 +7345,7 @@
         <v>2</v>
       </c>
       <c r="D64" s="11" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="E64" s="10">
         <v>3</v>
@@ -7398,7 +7395,7 @@
         <v>2</v>
       </c>
       <c r="D65" s="29" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="E65" s="28">
         <v>2</v>
@@ -7448,7 +7445,7 @@
         <v>2</v>
       </c>
       <c r="D66" s="91" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="E66" s="90">
         <v>2</v>
@@ -7498,7 +7495,7 @@
         <v>2</v>
       </c>
       <c r="D67" s="93" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="E67" s="92">
         <v>2</v>
@@ -7548,7 +7545,7 @@
         <v>2</v>
       </c>
       <c r="D68" s="13" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="E68" s="12">
         <v>2</v>
@@ -7598,7 +7595,7 @@
         <v>2</v>
       </c>
       <c r="D69" s="41" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="E69" s="40">
         <v>2</v>
@@ -7648,7 +7645,7 @@
         <v>2</v>
       </c>
       <c r="D70" s="73" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="E70" s="72">
         <v>2</v>
@@ -7698,7 +7695,7 @@
         <v>2</v>
       </c>
       <c r="D71" s="77" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="E71" s="76">
         <v>2</v>
@@ -7748,7 +7745,7 @@
         <v>2</v>
       </c>
       <c r="D72" s="95" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E72" s="94">
         <v>2</v>
@@ -7798,7 +7795,7 @@
         <v>2</v>
       </c>
       <c r="D73" s="97" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="E73" s="96">
         <v>2</v>
@@ -7848,7 +7845,7 @@
         <v>2</v>
       </c>
       <c r="D74" s="65" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="E74" s="64">
         <v>2</v>
@@ -7898,7 +7895,7 @@
         <v>2</v>
       </c>
       <c r="D75" s="99" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="E75" s="98">
         <v>2</v>
@@ -8896,7 +8893,7 @@
         <v>3</v>
       </c>
       <c r="D95" s="39" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="E95" s="38">
         <v>16</v>
@@ -8946,7 +8943,7 @@
         <v>3</v>
       </c>
       <c r="D96" s="73" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="E96" s="72">
         <v>4</v>
@@ -8996,7 +8993,7 @@
         <v>3</v>
       </c>
       <c r="D97" s="113" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="E97" s="112">
         <v>4</v>
@@ -9046,7 +9043,7 @@
         <v>3</v>
       </c>
       <c r="D98" s="39" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="E98" s="38">
         <v>3</v>
@@ -9096,7 +9093,7 @@
         <v>3</v>
       </c>
       <c r="D99" s="115" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="E99" s="114">
         <v>3</v>
@@ -9146,7 +9143,7 @@
         <v>3</v>
       </c>
       <c r="D100" s="89" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="E100" s="88">
         <v>3</v>
@@ -9196,7 +9193,7 @@
         <v>3</v>
       </c>
       <c r="D101" s="101" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="E101" s="100">
         <v>2</v>
@@ -9246,7 +9243,7 @@
         <v>3</v>
       </c>
       <c r="D102" s="91" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="E102" s="90">
         <v>2</v>
@@ -9296,7 +9293,7 @@
         <v>3</v>
       </c>
       <c r="D103" s="73" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="E103" s="72">
         <v>2</v>
@@ -9346,7 +9343,7 @@
         <v>3</v>
       </c>
       <c r="D104" s="29" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="E104" s="28">
         <v>2</v>
@@ -9396,7 +9393,7 @@
         <v>3</v>
       </c>
       <c r="D105" s="99" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="E105" s="98">
         <v>2</v>
@@ -9446,7 +9443,7 @@
         <v>3</v>
       </c>
       <c r="D106" s="51" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="E106" s="50">
         <v>2</v>
@@ -9496,7 +9493,7 @@
         <v>3</v>
       </c>
       <c r="D107" s="95" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="E107" s="94">
         <v>2</v>
@@ -9546,7 +9543,7 @@
         <v>3</v>
       </c>
       <c r="D108" s="39" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="E108" s="38">
         <v>2</v>
@@ -9596,7 +9593,7 @@
         <v>3</v>
       </c>
       <c r="D109" s="73" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="E109" s="72">
         <v>2</v>
@@ -9646,7 +9643,7 @@
         <v>3</v>
       </c>
       <c r="D110" s="101" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E110" s="100">
         <v>2</v>
@@ -9696,7 +9693,7 @@
         <v>3</v>
       </c>
       <c r="D111" s="117" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="E111" s="116">
         <v>2</v>
@@ -9746,7 +9743,7 @@
         <v>3</v>
       </c>
       <c r="D112" s="37" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="E112" s="36">
         <v>2</v>
@@ -10381,7 +10378,7 @@
       </c>
       <c r="P124" s="188"/>
     </row>
-    <row r="125" spans="1:16" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:16" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A125" s="242" t="s">
         <v>182</v>
       </c>
@@ -10392,7 +10389,7 @@
         <v>4</v>
       </c>
       <c r="D125" s="111" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="E125" s="110">
         <v>24</v>
@@ -10442,7 +10439,7 @@
         <v>4</v>
       </c>
       <c r="D126" s="121" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="E126" s="120">
         <v>18</v>
@@ -10492,7 +10489,7 @@
         <v>4</v>
       </c>
       <c r="D127" s="123" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="E127" s="122">
         <v>18</v>
@@ -10542,7 +10539,7 @@
         <v>4</v>
       </c>
       <c r="D128" s="125" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="E128" s="124">
         <v>7</v>
@@ -10592,7 +10589,7 @@
         <v>4</v>
       </c>
       <c r="D129" s="127" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="E129" s="126">
         <v>6</v>
@@ -10642,7 +10639,7 @@
         <v>4</v>
       </c>
       <c r="D130" s="79" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="E130" s="78">
         <v>5</v>
@@ -10692,7 +10689,7 @@
         <v>4</v>
       </c>
       <c r="D131" s="129" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="E131" s="128">
         <v>4</v>
@@ -10742,7 +10739,7 @@
         <v>4</v>
       </c>
       <c r="D132" s="37" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="E132" s="36">
         <v>4</v>
@@ -10792,7 +10789,7 @@
         <v>4</v>
       </c>
       <c r="D133" s="129" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="E133" s="128">
         <v>3</v>
@@ -10842,7 +10839,7 @@
         <v>4</v>
       </c>
       <c r="D134" s="3" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="E134" s="2">
         <v>3</v>
@@ -10892,7 +10889,7 @@
         <v>4</v>
       </c>
       <c r="D135" s="111" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E135" s="110">
         <v>3</v>
@@ -10942,7 +10939,7 @@
         <v>4</v>
       </c>
       <c r="D136" s="101" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="E136" s="100">
         <v>2</v>
@@ -11081,18 +11078,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:16" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A139" s="240" t="s">
         <v>198</v>
       </c>
       <c r="B139" s="106" t="s">
         <v>15</v>
       </c>
-      <c r="C139" s="106" t="s">
-        <v>199</v>
-      </c>
+      <c r="C139" s="106"/>
       <c r="D139" s="107" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="E139" s="106">
         <v>12</v>
@@ -11131,16 +11126,14 @@
     </row>
     <row r="140" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A140" s="240" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B140" s="106" t="s">
         <v>15</v>
       </c>
-      <c r="C140" s="106" t="s">
-        <v>199</v>
-      </c>
+      <c r="C140" s="106"/>
       <c r="D140" s="107" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="E140" s="106">
         <v>3</v>
@@ -11184,11 +11177,9 @@
       <c r="B141" s="106" t="s">
         <v>15</v>
       </c>
-      <c r="C141" s="106" t="s">
-        <v>199</v>
-      </c>
+      <c r="C141" s="106"/>
       <c r="D141" s="107" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="E141" s="106">
         <v>3</v>
@@ -11227,16 +11218,14 @@
     </row>
     <row r="142" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A142" s="240" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B142" s="106" t="s">
         <v>15</v>
       </c>
-      <c r="C142" s="106" t="s">
-        <v>199</v>
-      </c>
+      <c r="C142" s="106"/>
       <c r="D142" s="107" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="E142" s="106">
         <v>3</v>
@@ -11275,16 +11264,14 @@
     </row>
     <row r="143" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A143" s="240" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B143" s="106" t="s">
         <v>15</v>
       </c>
-      <c r="C143" s="106" t="s">
-        <v>199</v>
-      </c>
+      <c r="C143" s="106"/>
       <c r="D143" s="107" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="E143" s="106">
         <v>3</v>
@@ -11323,16 +11310,14 @@
     </row>
     <row r="144" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A144" s="240" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B144" s="106" t="s">
         <v>15</v>
       </c>
-      <c r="C144" s="106" t="s">
-        <v>199</v>
-      </c>
+      <c r="C144" s="106"/>
       <c r="D144" s="107" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E144" s="106">
         <v>3</v>
@@ -11371,16 +11356,14 @@
     </row>
     <row r="145" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A145" s="240" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B145" s="106" t="s">
         <v>15</v>
       </c>
-      <c r="C145" s="106" t="s">
-        <v>199</v>
-      </c>
+      <c r="C145" s="106"/>
       <c r="D145" s="107" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E145" s="106">
         <v>2</v>
@@ -11419,16 +11402,14 @@
     </row>
     <row r="146" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A146" s="240" t="s">
+        <v>204</v>
+      </c>
+      <c r="B146" s="106" t="s">
+        <v>15</v>
+      </c>
+      <c r="C146" s="106"/>
+      <c r="D146" s="107" t="s">
         <v>205</v>
-      </c>
-      <c r="B146" s="106" t="s">
-        <v>15</v>
-      </c>
-      <c r="C146" s="106" t="s">
-        <v>199</v>
-      </c>
-      <c r="D146" s="107" t="s">
-        <v>206</v>
       </c>
       <c r="E146" s="106">
         <v>1</v>
@@ -11467,16 +11448,14 @@
     </row>
     <row r="147" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A147" s="240" t="s">
+        <v>206</v>
+      </c>
+      <c r="B147" s="106" t="s">
+        <v>15</v>
+      </c>
+      <c r="C147" s="106"/>
+      <c r="D147" s="107" t="s">
         <v>207</v>
-      </c>
-      <c r="B147" s="106" t="s">
-        <v>15</v>
-      </c>
-      <c r="C147" s="106" t="s">
-        <v>199</v>
-      </c>
-      <c r="D147" s="107" t="s">
-        <v>208</v>
       </c>
       <c r="E147" s="106">
         <v>1</v>
@@ -11515,16 +11494,14 @@
     </row>
     <row r="148" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A148" s="240" t="s">
+        <v>208</v>
+      </c>
+      <c r="B148" s="106" t="s">
+        <v>15</v>
+      </c>
+      <c r="C148" s="106"/>
+      <c r="D148" s="107" t="s">
         <v>209</v>
-      </c>
-      <c r="B148" s="106" t="s">
-        <v>15</v>
-      </c>
-      <c r="C148" s="106" t="s">
-        <v>199</v>
-      </c>
-      <c r="D148" s="107" t="s">
-        <v>210</v>
       </c>
       <c r="E148" s="106">
         <v>1</v>
@@ -11563,16 +11540,14 @@
     </row>
     <row r="149" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A149" s="240" t="s">
+        <v>210</v>
+      </c>
+      <c r="B149" s="106" t="s">
+        <v>15</v>
+      </c>
+      <c r="C149" s="106"/>
+      <c r="D149" s="107" t="s">
         <v>211</v>
-      </c>
-      <c r="B149" s="106" t="s">
-        <v>15</v>
-      </c>
-      <c r="C149" s="106" t="s">
-        <v>199</v>
-      </c>
-      <c r="D149" s="107" t="s">
-        <v>212</v>
       </c>
       <c r="E149" s="106">
         <v>1</v>
@@ -11611,16 +11586,14 @@
     </row>
     <row r="150" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A150" s="222" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B150" s="72" t="s">
         <v>15</v>
       </c>
-      <c r="C150" s="72" t="s">
+      <c r="C150" s="72"/>
+      <c r="D150" s="73" t="s">
         <v>214</v>
-      </c>
-      <c r="D150" s="73" t="s">
-        <v>215</v>
       </c>
       <c r="E150" s="72">
         <v>1</v>
@@ -11661,14 +11634,14 @@
     </row>
     <row r="151" spans="1:16" ht="72" x14ac:dyDescent="0.3">
       <c r="A151" s="240" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B151" s="106" t="s">
         <v>15</v>
       </c>
       <c r="C151" s="106"/>
       <c r="D151" s="107" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="E151" s="106">
         <v>16</v>
@@ -11707,14 +11680,14 @@
     </row>
     <row r="152" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A152" s="189" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B152" s="6" t="s">
         <v>15</v>
       </c>
       <c r="C152" s="6"/>
       <c r="D152" s="7" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="E152" s="6">
         <v>6</v>
@@ -11755,14 +11728,14 @@
     </row>
     <row r="153" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A153" s="194" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B153" s="16" t="s">
         <v>15</v>
       </c>
       <c r="C153" s="16"/>
       <c r="D153" s="17" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="E153" s="16">
         <v>6</v>
@@ -11803,14 +11776,14 @@
     </row>
     <row r="154" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A154" s="240" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B154" s="106" t="s">
         <v>15</v>
       </c>
       <c r="C154" s="106"/>
       <c r="D154" s="107" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="E154" s="106">
         <v>6</v>
@@ -11849,14 +11822,14 @@
     </row>
     <row r="155" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A155" s="220" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B155" s="68" t="s">
         <v>15</v>
       </c>
       <c r="C155" s="68"/>
       <c r="D155" s="69" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="E155" s="68">
         <v>6</v>
@@ -11897,14 +11870,14 @@
     </row>
     <row r="156" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A156" s="240" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B156" s="106" t="s">
         <v>15</v>
       </c>
       <c r="C156" s="106"/>
       <c r="D156" s="107" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="E156" s="106">
         <v>6</v>
@@ -11943,14 +11916,14 @@
     </row>
     <row r="157" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A157" s="190" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B157" s="8" t="s">
         <v>15</v>
       </c>
       <c r="C157" s="8"/>
       <c r="D157" s="9" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="E157" s="8">
         <v>5</v>
@@ -11991,14 +11964,14 @@
     </row>
     <row r="158" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A158" s="211" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B158" s="50" t="s">
         <v>15</v>
       </c>
       <c r="C158" s="50"/>
       <c r="D158" s="51" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="E158" s="50">
         <v>5</v>
@@ -12037,16 +12010,16 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="159" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A159" s="235" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B159" s="96" t="s">
         <v>15</v>
       </c>
       <c r="C159" s="96"/>
       <c r="D159" s="97" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="E159" s="96">
         <v>4</v>
@@ -12087,14 +12060,14 @@
     </row>
     <row r="160" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A160" s="200" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B160" s="28" t="s">
         <v>15</v>
       </c>
       <c r="C160" s="28"/>
       <c r="D160" s="29" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E160" s="28">
         <v>4</v>
@@ -12135,14 +12108,14 @@
     </row>
     <row r="161" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A161" s="193" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B161" s="14" t="s">
         <v>15</v>
       </c>
       <c r="C161" s="14"/>
       <c r="D161" s="15" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="E161" s="14">
         <v>4</v>
@@ -12183,14 +12156,14 @@
     </row>
     <row r="162" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A162" s="222" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B162" s="72" t="s">
         <v>15</v>
       </c>
       <c r="C162" s="72"/>
       <c r="D162" s="73" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="E162" s="72">
         <v>4</v>
@@ -12231,14 +12204,14 @@
     </row>
     <row r="163" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A163" s="231" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B163" s="88" t="s">
         <v>15</v>
       </c>
       <c r="C163" s="88"/>
       <c r="D163" s="89" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="E163" s="88">
         <v>4</v>
@@ -12279,14 +12252,14 @@
     </row>
     <row r="164" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A164" s="240" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B164" s="106" t="s">
         <v>15</v>
       </c>
       <c r="C164" s="106"/>
       <c r="D164" s="107" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="E164" s="106">
         <v>4</v>
@@ -12325,14 +12298,14 @@
     </row>
     <row r="165" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A165" s="240" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B165" s="106" t="s">
         <v>15</v>
       </c>
       <c r="C165" s="106"/>
       <c r="D165" s="107" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="E165" s="106">
         <v>4</v>
@@ -12371,14 +12344,14 @@
     </row>
     <row r="166" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A166" s="210" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B166" s="48" t="s">
         <v>15</v>
       </c>
       <c r="C166" s="48"/>
       <c r="D166" s="49" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="E166" s="48">
         <v>4</v>
@@ -12419,14 +12392,14 @@
     </row>
     <row r="167" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A167" s="240" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B167" s="106" t="s">
         <v>15</v>
       </c>
       <c r="C167" s="106"/>
       <c r="D167" s="107" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="E167" s="106">
         <v>4</v>
@@ -12465,14 +12438,14 @@
     </row>
     <row r="168" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A168" s="206" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B168" s="40" t="s">
         <v>15</v>
       </c>
       <c r="C168" s="40"/>
       <c r="D168" s="41" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="E168" s="40">
         <v>3</v>
@@ -12513,14 +12486,14 @@
     </row>
     <row r="169" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A169" s="252" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B169" s="130" t="s">
         <v>15</v>
       </c>
       <c r="C169" s="130"/>
       <c r="D169" s="131" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="E169" s="130">
         <v>3</v>
@@ -12561,14 +12534,14 @@
     </row>
     <row r="170" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A170" s="194" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B170" s="16" t="s">
         <v>15</v>
       </c>
       <c r="C170" s="16"/>
       <c r="D170" s="17" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="E170" s="16">
         <v>3</v>
@@ -12616,7 +12589,7 @@
       </c>
       <c r="C171" s="132"/>
       <c r="D171" s="133" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="E171" s="132">
         <v>3</v>
@@ -12657,14 +12630,14 @@
     </row>
     <row r="172" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A172" s="239" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B172" s="104" t="s">
         <v>15</v>
       </c>
       <c r="C172" s="104"/>
       <c r="D172" s="105" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="E172" s="104">
         <v>3</v>
@@ -12705,14 +12678,14 @@
     </row>
     <row r="173" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A173" s="254" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B173" s="134" t="s">
         <v>15</v>
       </c>
       <c r="C173" s="134"/>
       <c r="D173" s="135" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="E173" s="134">
         <v>3</v>
@@ -12753,14 +12726,14 @@
     </row>
     <row r="174" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A174" s="204" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B174" s="36" t="s">
         <v>15</v>
       </c>
       <c r="C174" s="36"/>
       <c r="D174" s="37" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="E174" s="36">
         <v>3</v>
@@ -12801,14 +12774,14 @@
     </row>
     <row r="175" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A175" s="200" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B175" s="28" t="s">
         <v>15</v>
       </c>
       <c r="C175" s="28"/>
       <c r="D175" s="29" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="E175" s="28">
         <v>3</v>
@@ -12849,14 +12822,14 @@
     </row>
     <row r="176" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A176" s="240" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B176" s="106" t="s">
         <v>15</v>
       </c>
       <c r="C176" s="106"/>
       <c r="D176" s="107" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="E176" s="106">
         <v>3</v>
@@ -12895,14 +12868,14 @@
     </row>
     <row r="177" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A177" s="240" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B177" s="106" t="s">
         <v>15</v>
       </c>
       <c r="C177" s="106"/>
       <c r="D177" s="107" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="E177" s="106">
         <v>3</v>
@@ -12941,14 +12914,14 @@
     </row>
     <row r="178" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A178" s="212" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B178" s="52" t="s">
         <v>15</v>
       </c>
       <c r="C178" s="52"/>
       <c r="D178" s="53" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="E178" s="52">
         <v>3</v>
@@ -12989,14 +12962,14 @@
     </row>
     <row r="179" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A179" s="255" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B179" s="136" t="s">
         <v>15</v>
       </c>
       <c r="C179" s="136"/>
       <c r="D179" s="137" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="E179" s="136">
         <v>3</v>
@@ -13037,14 +13010,14 @@
     </row>
     <row r="180" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A180" s="240" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B180" s="106" t="s">
         <v>15</v>
       </c>
       <c r="C180" s="106"/>
       <c r="D180" s="107" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="E180" s="106">
         <v>3</v>
@@ -13083,14 +13056,14 @@
     </row>
     <row r="181" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A181" s="209" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B181" s="46" t="s">
         <v>15</v>
       </c>
       <c r="C181" s="46"/>
       <c r="D181" s="47" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="E181" s="46">
         <v>3</v>
@@ -13131,14 +13104,14 @@
     </row>
     <row r="182" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A182" s="228" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B182" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C182" s="2"/>
       <c r="D182" s="3" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="E182" s="2">
         <v>3</v>
@@ -13179,14 +13152,14 @@
     </row>
     <row r="183" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A183" s="240" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B183" s="106" t="s">
         <v>15</v>
       </c>
       <c r="C183" s="106"/>
       <c r="D183" s="107" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="E183" s="106">
         <v>3</v>
@@ -13225,14 +13198,14 @@
     </row>
     <row r="184" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A184" s="256" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B184" s="138" t="s">
         <v>15</v>
       </c>
       <c r="C184" s="138"/>
       <c r="D184" s="139" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="E184" s="138">
         <v>2</v>
@@ -13273,14 +13246,14 @@
     </row>
     <row r="185" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A185" s="207" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B185" s="42" t="s">
         <v>15</v>
       </c>
       <c r="C185" s="42"/>
       <c r="D185" s="43" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="E185" s="42">
         <v>2</v>
@@ -13321,14 +13294,14 @@
     </row>
     <row r="186" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A186" s="242" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B186" s="110" t="s">
         <v>15</v>
       </c>
       <c r="C186" s="110"/>
       <c r="D186" s="111" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="E186" s="110">
         <v>2</v>
@@ -13369,14 +13342,14 @@
     </row>
     <row r="187" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A187" s="257" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B187" s="140" t="s">
         <v>15</v>
       </c>
       <c r="C187" s="140"/>
       <c r="D187" s="141" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="E187" s="140">
         <v>2</v>
@@ -13417,14 +13390,14 @@
     </row>
     <row r="188" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A188" s="194" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B188" s="16" t="s">
         <v>15</v>
       </c>
       <c r="C188" s="16"/>
       <c r="D188" s="17" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="E188" s="16">
         <v>2</v>
@@ -13465,14 +13438,14 @@
     </row>
     <row r="189" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A189" s="258" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B189" s="142" t="s">
         <v>15</v>
       </c>
       <c r="C189" s="142"/>
       <c r="D189" s="143" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="E189" s="142">
         <v>2</v>
@@ -13513,14 +13486,14 @@
     </row>
     <row r="190" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A190" s="239" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B190" s="104" t="s">
         <v>15</v>
       </c>
       <c r="C190" s="104"/>
       <c r="D190" s="105" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="E190" s="104">
         <v>2</v>
@@ -13561,14 +13534,14 @@
     </row>
     <row r="191" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A191" s="259" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B191" s="144" t="s">
         <v>15</v>
       </c>
       <c r="C191" s="144"/>
       <c r="D191" s="145" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="E191" s="144">
         <v>2</v>
@@ -13609,14 +13582,14 @@
     </row>
     <row r="192" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A192" s="232" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B192" s="90" t="s">
         <v>15</v>
       </c>
       <c r="C192" s="90"/>
       <c r="D192" s="91" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="E192" s="90">
         <v>2</v>
@@ -13657,14 +13630,14 @@
     </row>
     <row r="193" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A193" s="256" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B193" s="138" t="s">
         <v>15</v>
       </c>
       <c r="C193" s="138"/>
       <c r="D193" s="139" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="E193" s="138">
         <v>2</v>
@@ -13705,14 +13678,14 @@
     </row>
     <row r="194" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A194" s="240" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B194" s="106" t="s">
         <v>15</v>
       </c>
       <c r="C194" s="106"/>
       <c r="D194" s="107" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="E194" s="106">
         <v>2</v>
@@ -13751,14 +13724,14 @@
     </row>
     <row r="195" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A195" s="204" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B195" s="36" t="s">
         <v>15</v>
       </c>
       <c r="C195" s="36"/>
       <c r="D195" s="37" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="E195" s="36">
         <v>2</v>
@@ -13799,14 +13772,14 @@
     </row>
     <row r="196" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A196" s="260" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B196" s="146" t="s">
         <v>15</v>
       </c>
       <c r="C196" s="146"/>
       <c r="D196" s="147" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="E196" s="146">
         <v>2</v>
@@ -13847,14 +13820,14 @@
     </row>
     <row r="197" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A197" s="204" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B197" s="36" t="s">
         <v>15</v>
       </c>
       <c r="C197" s="36"/>
       <c r="D197" s="37" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="E197" s="36">
         <v>2</v>
@@ -13895,14 +13868,14 @@
     </row>
     <row r="198" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A198" s="237" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B198" s="100" t="s">
         <v>15</v>
       </c>
       <c r="C198" s="100"/>
       <c r="D198" s="101" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="E198" s="100">
         <v>2</v>
@@ -13943,14 +13916,14 @@
     </row>
     <row r="199" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A199" s="240" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B199" s="106" t="s">
         <v>15</v>
       </c>
       <c r="C199" s="106"/>
       <c r="D199" s="107" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="E199" s="106">
         <v>2</v>
@@ -13989,14 +13962,14 @@
     </row>
     <row r="200" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A200" s="222" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B200" s="72" t="s">
         <v>15</v>
       </c>
       <c r="C200" s="72"/>
       <c r="D200" s="73" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="E200" s="72">
         <v>2</v>
@@ -14037,14 +14010,14 @@
     </row>
     <row r="201" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A201" s="222" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B201" s="72" t="s">
         <v>15</v>
       </c>
       <c r="C201" s="72"/>
       <c r="D201" s="73" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E201" s="72">
         <v>1</v>
@@ -14085,14 +14058,14 @@
     </row>
     <row r="202" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A202" s="260" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B202" s="146" t="s">
         <v>15</v>
       </c>
       <c r="C202" s="146"/>
       <c r="D202" s="147" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E202" s="146">
         <v>1</v>
@@ -14133,14 +14106,14 @@
     </row>
     <row r="203" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A203" s="222" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B203" s="72" t="s">
         <v>15</v>
       </c>
       <c r="C203" s="72"/>
       <c r="D203" s="73" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E203" s="72">
         <v>1</v>
@@ -14181,14 +14154,14 @@
     </row>
     <row r="204" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A204" s="261" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B204" s="148" t="s">
         <v>15</v>
       </c>
       <c r="C204" s="148"/>
       <c r="D204" s="149" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E204" s="148">
         <v>1</v>
@@ -14229,14 +14202,14 @@
     </row>
     <row r="205" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A205" s="222" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B205" s="72" t="s">
         <v>15</v>
       </c>
       <c r="C205" s="72"/>
       <c r="D205" s="73" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E205" s="72">
         <v>1</v>
@@ -14277,14 +14250,14 @@
     </row>
     <row r="206" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A206" s="239" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B206" s="104" t="s">
         <v>15</v>
       </c>
       <c r="C206" s="104"/>
       <c r="D206" s="105" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E206" s="104">
         <v>1</v>
@@ -14325,14 +14298,14 @@
     </row>
     <row r="207" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A207" s="224" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B207" s="76" t="s">
         <v>15</v>
       </c>
       <c r="C207" s="76"/>
       <c r="D207" s="77" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E207" s="76">
         <v>1</v>
@@ -14373,14 +14346,14 @@
     </row>
     <row r="208" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A208" s="237" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B208" s="100" t="s">
         <v>15</v>
       </c>
       <c r="C208" s="100"/>
       <c r="D208" s="101" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E208" s="100">
         <v>1</v>
@@ -14421,14 +14394,14 @@
     </row>
     <row r="209" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A209" s="213" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B209" s="54" t="s">
         <v>15</v>
       </c>
       <c r="C209" s="54"/>
       <c r="D209" s="55" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E209" s="54">
         <v>1</v>
@@ -14469,14 +14442,14 @@
     </row>
     <row r="210" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A210" s="239" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B210" s="104" t="s">
         <v>15</v>
       </c>
       <c r="C210" s="104"/>
       <c r="D210" s="105" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E210" s="104">
         <v>1</v>
@@ -14517,14 +14490,14 @@
     </row>
     <row r="211" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A211" s="222" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B211" s="72" t="s">
         <v>15</v>
       </c>
       <c r="C211" s="72"/>
       <c r="D211" s="73" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E211" s="72">
         <v>1</v>
@@ -14565,14 +14538,14 @@
     </row>
     <row r="212" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A212" s="232" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B212" s="90" t="s">
         <v>15</v>
       </c>
       <c r="C212" s="90"/>
       <c r="D212" s="91" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E212" s="90">
         <v>1</v>
@@ -14613,14 +14586,14 @@
     </row>
     <row r="213" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A213" s="207" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B213" s="42" t="s">
         <v>15</v>
       </c>
       <c r="C213" s="42"/>
       <c r="D213" s="43" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E213" s="42">
         <v>1</v>
@@ -14661,14 +14634,14 @@
     </row>
     <row r="214" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A214" s="211" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B214" s="50" t="s">
         <v>15</v>
       </c>
       <c r="C214" s="50"/>
       <c r="D214" s="51" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E214" s="50">
         <v>1</v>
@@ -14709,14 +14682,14 @@
     </row>
     <row r="215" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A215" s="240" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B215" s="106" t="s">
         <v>15</v>
       </c>
       <c r="C215" s="106"/>
       <c r="D215" s="107" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E215" s="106">
         <v>1</v>
@@ -14755,14 +14728,14 @@
     </row>
     <row r="216" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A216" s="240" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B216" s="106" t="s">
         <v>15</v>
       </c>
       <c r="C216" s="106"/>
       <c r="D216" s="107" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E216" s="106">
         <v>1</v>
@@ -14801,14 +14774,14 @@
     </row>
     <row r="217" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A217" s="224" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B217" s="76" t="s">
         <v>15</v>
       </c>
       <c r="C217" s="76"/>
       <c r="D217" s="77" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E217" s="76">
         <v>1</v>
@@ -14849,14 +14822,14 @@
     </row>
     <row r="218" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A218" s="240" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B218" s="106" t="s">
         <v>15</v>
       </c>
       <c r="C218" s="106"/>
       <c r="D218" s="107" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E218" s="106">
         <v>1</v>
@@ -14895,14 +14868,14 @@
     </row>
     <row r="219" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A219" s="240" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B219" s="106" t="s">
         <v>15</v>
       </c>
       <c r="C219" s="106"/>
       <c r="D219" s="107" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E219" s="106">
         <v>1</v>
@@ -14941,14 +14914,14 @@
     </row>
     <row r="220" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A220" s="241" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B220" s="108" t="s">
         <v>15</v>
       </c>
       <c r="C220" s="108"/>
       <c r="D220" s="109" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E220" s="108">
         <v>1</v>
@@ -14989,14 +14962,14 @@
     </row>
     <row r="221" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A221" s="213" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B221" s="54" t="s">
         <v>15</v>
       </c>
       <c r="C221" s="54"/>
       <c r="D221" s="55" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E221" s="54">
         <v>1</v>
@@ -15037,14 +15010,14 @@
     </row>
     <row r="222" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A222" s="213" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B222" s="54" t="s">
         <v>15</v>
       </c>
       <c r="C222" s="54"/>
       <c r="D222" s="55" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E222" s="54">
         <v>1</v>
@@ -15085,14 +15058,14 @@
     </row>
     <row r="223" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A223" s="209" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B223" s="46" t="s">
         <v>15</v>
       </c>
       <c r="C223" s="46"/>
       <c r="D223" s="47" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E223" s="46">
         <v>1</v>
@@ -15133,14 +15106,14 @@
     </row>
     <row r="224" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A224" s="210" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B224" s="48" t="s">
         <v>15</v>
       </c>
       <c r="C224" s="48"/>
       <c r="D224" s="49" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E224" s="48">
         <v>1</v>
@@ -15181,14 +15154,14 @@
     </row>
     <row r="225" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A225" s="205" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B225" s="38" t="s">
         <v>15</v>
       </c>
       <c r="C225" s="38"/>
       <c r="D225" s="39" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E225" s="38">
         <v>1</v>
@@ -15229,14 +15202,14 @@
     </row>
     <row r="226" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A226" s="222" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B226" s="72" t="s">
         <v>15</v>
       </c>
       <c r="C226" s="72"/>
       <c r="D226" s="73" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E226" s="72">
         <v>1</v>
@@ -15277,14 +15250,14 @@
     </row>
     <row r="227" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A227" s="194" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B227" s="16" t="s">
         <v>15</v>
       </c>
       <c r="C227" s="16"/>
       <c r="D227" s="17" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E227" s="16">
         <v>1</v>
@@ -15325,14 +15298,14 @@
     </row>
     <row r="228" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A228" s="211" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B228" s="50" t="s">
         <v>15</v>
       </c>
       <c r="C228" s="50"/>
       <c r="D228" s="51" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E228" s="50">
         <v>1</v>
@@ -15373,14 +15346,14 @@
     </row>
     <row r="229" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A229" s="222" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B229" s="72" t="s">
         <v>15</v>
       </c>
       <c r="C229" s="72"/>
       <c r="D229" s="73" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E229" s="72">
         <v>1</v>
@@ -15421,14 +15394,14 @@
     </row>
     <row r="230" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A230" s="194" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B230" s="16" t="s">
         <v>15</v>
       </c>
       <c r="C230" s="16"/>
       <c r="D230" s="17" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E230" s="16">
         <v>1</v>
@@ -15469,14 +15442,14 @@
     </row>
     <row r="231" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A231" s="224" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B231" s="76" t="s">
         <v>15</v>
       </c>
       <c r="C231" s="76"/>
       <c r="D231" s="77" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E231" s="76">
         <v>1</v>
@@ -15517,14 +15490,14 @@
     </row>
     <row r="232" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A232" s="211" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B232" s="50" t="s">
         <v>15</v>
       </c>
       <c r="C232" s="50"/>
       <c r="D232" s="51" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E232" s="50">
         <v>1</v>
@@ -15565,14 +15538,14 @@
     </row>
     <row r="233" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A233" s="240" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B233" s="106" t="s">
         <v>15</v>
       </c>
       <c r="C233" s="106"/>
       <c r="D233" s="107" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E233" s="106">
         <v>1</v>
@@ -15611,14 +15584,14 @@
     </row>
     <row r="234" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A234" s="213" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B234" s="54" t="s">
         <v>15</v>
       </c>
       <c r="C234" s="54"/>
       <c r="D234" s="55" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E234" s="54">
         <v>1</v>
@@ -15659,14 +15632,14 @@
     </row>
     <row r="235" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A235" s="240" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B235" s="106" t="s">
         <v>15</v>
       </c>
       <c r="C235" s="106"/>
       <c r="D235" s="107" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E235" s="106">
         <v>1</v>
@@ -15705,14 +15678,14 @@
     </row>
     <row r="236" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A236" s="209" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B236" s="46" t="s">
         <v>15</v>
       </c>
       <c r="C236" s="46"/>
       <c r="D236" s="47" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E236" s="46">
         <v>1</v>
@@ -15753,14 +15726,14 @@
     </row>
     <row r="237" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A237" s="237" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B237" s="100" t="s">
         <v>15</v>
       </c>
       <c r="C237" s="100"/>
       <c r="D237" s="101" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E237" s="100">
         <v>1</v>
@@ -15801,16 +15774,16 @@
     </row>
     <row r="238" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A238" s="192" t="s">
+        <v>323</v>
+      </c>
+      <c r="B238" s="12" t="s">
         <v>324</v>
       </c>
-      <c r="B238" s="12" t="s">
-        <v>325</v>
-      </c>
       <c r="C238" s="12">
         <v>1</v>
       </c>
       <c r="D238" s="13" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E238" s="12">
         <v>6</v>
@@ -15851,16 +15824,16 @@
     </row>
     <row r="239" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A239" s="227" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B239" s="82" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C239" s="82">
         <v>2</v>
       </c>
       <c r="D239" s="83" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="E239" s="82">
         <v>9</v>
@@ -15901,16 +15874,16 @@
     </row>
     <row r="240" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A240" s="262" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B240" s="150" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C240" s="150">
         <v>2</v>
       </c>
       <c r="D240" s="151" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="E240" s="150">
         <v>8</v>
@@ -15951,16 +15924,16 @@
     </row>
     <row r="241" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A241" s="263" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B241" s="152" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C241" s="152">
         <v>2</v>
       </c>
       <c r="D241" s="153" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="E241" s="152">
         <v>7</v>
@@ -16001,16 +15974,16 @@
     </row>
     <row r="242" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A242" s="264" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B242" s="154" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C242" s="154">
         <v>2</v>
       </c>
       <c r="D242" s="155" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="E242" s="154">
         <v>6</v>
@@ -16051,16 +16024,16 @@
     </row>
     <row r="243" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A243" s="219" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B243" s="66" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C243" s="66">
         <v>2</v>
       </c>
       <c r="D243" s="67" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="E243" s="66">
         <v>6</v>
@@ -16101,16 +16074,16 @@
     </row>
     <row r="244" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A244" s="265" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B244" s="156" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C244" s="156">
         <v>2</v>
       </c>
       <c r="D244" s="157" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="E244" s="156">
         <v>6</v>
@@ -16151,16 +16124,16 @@
     </row>
     <row r="245" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A245" s="266" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B245" s="158" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C245" s="158">
         <v>2</v>
       </c>
       <c r="D245" s="159" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="E245" s="158">
         <v>5</v>
@@ -16201,16 +16174,16 @@
     </row>
     <row r="246" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A246" s="267" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B246" s="160" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C246" s="160">
         <v>2</v>
       </c>
       <c r="D246" s="161" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="E246" s="160">
         <v>4</v>
@@ -16251,16 +16224,16 @@
     </row>
     <row r="247" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A247" s="225" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B247" s="78" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C247" s="78">
         <v>2</v>
       </c>
       <c r="D247" s="79" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="E247" s="78">
         <v>3</v>
@@ -16301,16 +16274,16 @@
     </row>
     <row r="248" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A248" s="203" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B248" s="34" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C248" s="34">
         <v>2</v>
       </c>
       <c r="D248" s="35" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="E248" s="34">
         <v>2</v>
@@ -16351,16 +16324,16 @@
     </row>
     <row r="249" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A249" s="268" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B249" s="162" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C249" s="162">
         <v>2</v>
       </c>
       <c r="D249" s="163" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="E249" s="162">
         <v>2</v>
@@ -16401,16 +16374,16 @@
     </row>
     <row r="250" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A250" s="208" t="s">
+        <v>336</v>
+      </c>
+      <c r="B250" s="44" t="s">
+        <v>324</v>
+      </c>
+      <c r="C250" s="44">
+        <v>2</v>
+      </c>
+      <c r="D250" s="45" t="s">
         <v>337</v>
-      </c>
-      <c r="B250" s="44" t="s">
-        <v>325</v>
-      </c>
-      <c r="C250" s="44">
-        <v>2</v>
-      </c>
-      <c r="D250" s="45" t="s">
-        <v>338</v>
       </c>
       <c r="E250" s="44">
         <v>1</v>
@@ -16451,16 +16424,16 @@
     </row>
     <row r="251" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A251" s="203" t="s">
+        <v>338</v>
+      </c>
+      <c r="B251" s="34" t="s">
+        <v>324</v>
+      </c>
+      <c r="C251" s="34">
+        <v>2</v>
+      </c>
+      <c r="D251" s="35" t="s">
         <v>339</v>
-      </c>
-      <c r="B251" s="34" t="s">
-        <v>325</v>
-      </c>
-      <c r="C251" s="34">
-        <v>2</v>
-      </c>
-      <c r="D251" s="35" t="s">
-        <v>340</v>
       </c>
       <c r="E251" s="34">
         <v>1</v>
@@ -16501,16 +16474,16 @@
     </row>
     <row r="252" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A252" s="194" t="s">
+        <v>340</v>
+      </c>
+      <c r="B252" s="16" t="s">
+        <v>324</v>
+      </c>
+      <c r="C252" s="16">
+        <v>2</v>
+      </c>
+      <c r="D252" s="17" t="s">
         <v>341</v>
-      </c>
-      <c r="B252" s="16" t="s">
-        <v>325</v>
-      </c>
-      <c r="C252" s="16">
-        <v>2</v>
-      </c>
-      <c r="D252" s="17" t="s">
-        <v>342</v>
       </c>
       <c r="E252" s="16">
         <v>1</v>
@@ -16551,16 +16524,16 @@
     </row>
     <row r="253" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A253" s="242" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B253" s="110" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C253" s="110">
         <v>3</v>
       </c>
       <c r="D253" s="111" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="E253" s="110">
         <v>3</v>
@@ -16601,16 +16574,16 @@
     </row>
     <row r="254" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A254" s="237" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B254" s="100" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C254" s="100">
         <v>3</v>
       </c>
       <c r="D254" s="101" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="E254" s="100">
         <v>2</v>
@@ -16651,16 +16624,16 @@
     </row>
     <row r="255" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A255" s="235" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B255" s="96" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C255" s="96">
         <v>4</v>
       </c>
       <c r="D255" s="97" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="E255" s="96">
         <v>7</v>
@@ -16699,18 +16672,18 @@
         <v>0.3125</v>
       </c>
     </row>
-    <row r="256" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A256" s="194" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B256" s="16" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C256" s="16">
         <v>4</v>
       </c>
       <c r="D256" s="17" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="E256" s="16">
         <v>4</v>
@@ -16751,16 +16724,16 @@
     </row>
     <row r="257" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A257" s="269" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B257" s="164" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C257" s="164">
         <v>4</v>
       </c>
       <c r="D257" s="165" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="E257" s="164">
         <v>3</v>
@@ -16801,16 +16774,16 @@
     </row>
     <row r="258" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A258" s="242" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B258" s="110" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C258" s="110">
         <v>4</v>
       </c>
       <c r="D258" s="111" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E258" s="110">
         <v>1</v>
@@ -16851,16 +16824,16 @@
     </row>
     <row r="259" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A259" s="205" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B259" s="38" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C259" s="38">
         <v>4</v>
       </c>
       <c r="D259" s="39" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E259" s="38">
         <v>1</v>
@@ -16901,16 +16874,16 @@
     </row>
     <row r="260" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A260" s="242" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B260" s="110" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C260" s="110">
         <v>4</v>
       </c>
       <c r="D260" s="111" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="E260" s="110">
         <v>1</v>
@@ -16951,14 +16924,14 @@
     </row>
     <row r="261" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A261" s="192" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B261" s="12" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C261" s="12"/>
       <c r="D261" s="13" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="E261" s="12">
         <v>8</v>
@@ -16999,14 +16972,14 @@
     </row>
     <row r="262" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A262" s="270" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B262" s="166" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C262" s="166"/>
       <c r="D262" s="167" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="E262" s="166">
         <v>8</v>
@@ -17047,14 +17020,14 @@
     </row>
     <row r="263" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A263" s="271" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B263" s="168" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C263" s="168"/>
       <c r="D263" s="169" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="E263" s="168">
         <v>6</v>
@@ -17095,14 +17068,14 @@
     </row>
     <row r="264" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A264" s="272" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B264" s="170" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C264" s="170"/>
       <c r="D264" s="171" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="E264" s="170">
         <v>3</v>
@@ -17143,14 +17116,14 @@
     </row>
     <row r="265" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A265" s="248" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B265" s="122" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C265" s="122"/>
       <c r="D265" s="123" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E265" s="122">
         <v>3</v>
@@ -17191,14 +17164,14 @@
     </row>
     <row r="266" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A266" s="193" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B266" s="14" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C266" s="14"/>
       <c r="D266" s="15" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E266" s="14">
         <v>3</v>
@@ -17239,14 +17212,14 @@
     </row>
     <row r="267" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A267" s="207" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B267" s="42" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C267" s="42"/>
       <c r="D267" s="43" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="E267" s="42">
         <v>2</v>
@@ -17287,14 +17260,14 @@
     </row>
     <row r="268" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A268" s="273" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B268" s="172" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C268" s="172"/>
       <c r="D268" s="173" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="E268" s="172">
         <v>2</v>
@@ -17335,14 +17308,14 @@
     </row>
     <row r="269" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A269" s="236" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B269" s="98" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C269" s="98"/>
       <c r="D269" s="99" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="E269" s="98">
         <v>2</v>
@@ -17383,14 +17356,14 @@
     </row>
     <row r="270" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A270" s="274" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B270" s="174" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C270" s="174"/>
       <c r="D270" s="175" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="E270" s="174">
         <v>2</v>
@@ -17431,14 +17404,14 @@
     </row>
     <row r="271" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A271" s="258" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B271" s="142" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C271" s="142"/>
       <c r="D271" s="143" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="E271" s="142">
         <v>2</v>
@@ -17479,14 +17452,14 @@
     </row>
     <row r="272" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A272" s="222" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B272" s="72" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C272" s="72"/>
       <c r="D272" s="73" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="E272" s="72">
         <v>1</v>
@@ -17527,14 +17500,14 @@
     </row>
     <row r="273" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A273" s="194" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B273" s="16" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C273" s="16"/>
       <c r="D273" s="17" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="E273" s="16">
         <v>1</v>
@@ -17575,14 +17548,14 @@
     </row>
     <row r="274" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A274" s="241" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B274" s="108" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C274" s="108"/>
       <c r="D274" s="109" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="E274" s="108">
         <v>1</v>
@@ -17623,14 +17596,14 @@
     </row>
     <row r="275" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A275" s="232" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B275" s="90" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C275" s="90"/>
       <c r="D275" s="91" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E275" s="90">
         <v>1</v>
@@ -17671,14 +17644,14 @@
     </row>
     <row r="276" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A276" s="194" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B276" s="16" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C276" s="16"/>
       <c r="D276" s="17" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="E276" s="16">
         <v>1</v>
@@ -17719,14 +17692,14 @@
     </row>
     <row r="277" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A277" s="224" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B277" s="76" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C277" s="76"/>
       <c r="D277" s="77" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E277" s="76">
         <v>1</v>
@@ -17767,14 +17740,14 @@
     </row>
     <row r="278" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A278" s="204" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B278" s="36" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C278" s="36"/>
       <c r="D278" s="37" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E278" s="36">
         <v>1</v>
@@ -17815,14 +17788,14 @@
     </row>
     <row r="279" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A279" s="222" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B279" s="72" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C279" s="72"/>
       <c r="D279" s="73" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="E279" s="72">
         <v>1</v>
@@ -17863,14 +17836,14 @@
     </row>
     <row r="280" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A280" s="202" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B280" s="32" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C280" s="32"/>
       <c r="D280" s="33" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E280" s="32">
         <v>1</v>
@@ -17911,14 +17884,14 @@
     </row>
     <row r="281" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A281" s="275" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B281" s="176" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C281" s="176"/>
       <c r="D281" s="177" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="E281" s="176">
         <v>1</v>
@@ -17959,14 +17932,14 @@
     </row>
     <row r="282" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A282" s="194" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B282" s="16" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C282" s="16"/>
       <c r="D282" s="17" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E282" s="16">
         <v>1</v>
@@ -18007,16 +17980,16 @@
     </row>
     <row r="283" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A283" s="276" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B283" s="178" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C283" s="178">
         <v>2</v>
       </c>
       <c r="D283" s="179" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="E283" s="178">
         <v>4</v>
@@ -18057,16 +18030,16 @@
     </row>
     <row r="284" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A284" s="197" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B284" s="22" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C284" s="22">
         <v>2</v>
       </c>
       <c r="D284" s="23" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="E284" s="22">
         <v>4</v>
@@ -18107,14 +18080,14 @@
     </row>
     <row r="285" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A285" s="254" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B285" s="134" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C285" s="134"/>
       <c r="D285" s="135" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="E285" s="134">
         <v>3</v>
@@ -18155,14 +18128,14 @@
     </row>
     <row r="286" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A286" s="240" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B286" s="106" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C286" s="106"/>
       <c r="D286" s="107" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E286" s="106">
         <v>1</v>
@@ -18201,14 +18174,14 @@
     </row>
     <row r="287" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A287" s="277" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B287" s="278" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C287" s="278"/>
       <c r="D287" s="279" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="E287" s="278">
         <v>1</v>
@@ -18248,7 +18221,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:P287"/>
+  <autoFilter ref="A1:P287" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <conditionalFormatting sqref="P2:P287">
     <cfRule type="colorScale" priority="1">
       <colorScale>

</xml_diff>